<commit_message>
delete 3 files, change parse
</commit_message>
<xml_diff>
--- a/data/small.xlsx
+++ b/data/small.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2416,7 +2416,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2447,6 +2447,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2465,9 +2473,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2476,10 +2485,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2813,7 +2823,7 @@
   <dimension ref="A1:J200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J200"/>
+      <selection sqref="A1:J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4380,7 +4390,7 @@
       <c r="E50" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="F50" s="6" t="s">
+      <c r="F50" s="7" t="s">
         <v>224</v>
       </c>
       <c r="G50" s="5" t="s">
@@ -4392,7 +4402,7 @@
       <c r="I50" s="5">
         <v>123</v>
       </c>
-      <c r="J50" s="7">
+      <c r="J50" s="6">
         <v>40781.633333333331</v>
       </c>
     </row>
@@ -4404,11 +4414,11 @@
       <c r="E51" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="F51" s="6"/>
+      <c r="F51" s="7"/>
       <c r="G51" s="5"/>
       <c r="H51" s="5"/>
       <c r="I51" s="5"/>
-      <c r="J51" s="7"/>
+      <c r="J51" s="6"/>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="1" t="s">
@@ -6680,7 +6690,7 @@
       <c r="E123" s="1" t="s">
         <v>518</v>
       </c>
-      <c r="F123" s="6" t="s">
+      <c r="F123" s="7" t="s">
         <v>519</v>
       </c>
       <c r="G123" s="5" t="s">
@@ -6692,7 +6702,7 @@
       <c r="I123" s="5">
         <v>279</v>
       </c>
-      <c r="J123" s="7">
+      <c r="J123" s="6">
         <v>40781.661805555559</v>
       </c>
     </row>
@@ -6704,11 +6714,11 @@
       <c r="E124" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="F124" s="6"/>
+      <c r="F124" s="7"/>
       <c r="G124" s="5"/>
       <c r="H124" s="5"/>
       <c r="I124" s="5"/>
-      <c r="J124" s="7"/>
+      <c r="J124" s="6"/>
     </row>
     <row r="125" spans="1:10">
       <c r="A125" s="5" t="s">
@@ -6726,7 +6736,7 @@
       <c r="E125" s="1" t="s">
         <v>521</v>
       </c>
-      <c r="F125" s="6" t="s">
+      <c r="F125" s="7" t="s">
         <v>522</v>
       </c>
       <c r="G125" s="5" t="s">
@@ -6738,7 +6748,7 @@
       <c r="I125" s="5">
         <v>279</v>
       </c>
-      <c r="J125" s="7">
+      <c r="J125" s="6">
         <v>40781.661805555559</v>
       </c>
     </row>
@@ -6750,11 +6760,11 @@
       <c r="E126" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="F126" s="6"/>
+      <c r="F126" s="7"/>
       <c r="G126" s="5"/>
       <c r="H126" s="5"/>
       <c r="I126" s="5"/>
-      <c r="J126" s="7"/>
+      <c r="J126" s="6"/>
     </row>
     <row r="127" spans="1:10">
       <c r="A127" s="1" t="s">
@@ -6804,7 +6814,7 @@
       <c r="E128" s="1" t="s">
         <v>528</v>
       </c>
-      <c r="F128" s="6" t="s">
+      <c r="F128" s="7" t="s">
         <v>529</v>
       </c>
       <c r="G128" s="5" t="s">
@@ -6816,7 +6826,7 @@
       <c r="I128" s="5">
         <v>279</v>
       </c>
-      <c r="J128" s="7">
+      <c r="J128" s="6">
         <v>40781.662499999999</v>
       </c>
     </row>
@@ -6828,11 +6838,11 @@
       <c r="E129" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="F129" s="6"/>
+      <c r="F129" s="7"/>
       <c r="G129" s="5"/>
       <c r="H129" s="5"/>
       <c r="I129" s="5"/>
-      <c r="J129" s="7"/>
+      <c r="J129" s="6"/>
     </row>
     <row r="130" spans="1:10">
       <c r="A130" s="1" t="s">
@@ -8818,7 +8828,7 @@
       <c r="E192" s="1" t="s">
         <v>770</v>
       </c>
-      <c r="F192" s="6" t="s">
+      <c r="F192" s="7" t="s">
         <v>771</v>
       </c>
       <c r="G192" s="5" t="s">
@@ -8830,7 +8840,7 @@
       <c r="I192" s="5">
         <v>3931</v>
       </c>
-      <c r="J192" s="7">
+      <c r="J192" s="6">
         <v>40781.681944444441</v>
       </c>
     </row>
@@ -8842,11 +8852,11 @@
       <c r="E193" s="1" t="s">
         <v>772</v>
       </c>
-      <c r="F193" s="6"/>
+      <c r="F193" s="7"/>
       <c r="G193" s="5"/>
       <c r="H193" s="5"/>
       <c r="I193" s="5"/>
-      <c r="J193" s="7"/>
+      <c r="J193" s="6"/>
     </row>
     <row r="194" spans="1:10">
       <c r="A194" s="5" t="s">
@@ -8864,7 +8874,7 @@
       <c r="E194" s="1" t="s">
         <v>775</v>
       </c>
-      <c r="F194" s="6" t="s">
+      <c r="F194" s="7" t="s">
         <v>776</v>
       </c>
       <c r="G194" s="5" t="s">
@@ -8876,7 +8886,7 @@
       <c r="I194" s="5">
         <v>5291</v>
       </c>
-      <c r="J194" s="7">
+      <c r="J194" s="6">
         <v>40781.682638888888</v>
       </c>
     </row>
@@ -8888,11 +8898,11 @@
       <c r="E195" s="1" t="s">
         <v>778</v>
       </c>
-      <c r="F195" s="6"/>
+      <c r="F195" s="7"/>
       <c r="G195" s="5"/>
       <c r="H195" s="5"/>
       <c r="I195" s="5"/>
-      <c r="J195" s="7"/>
+      <c r="J195" s="6"/>
     </row>
     <row r="196" spans="1:10">
       <c r="A196" s="1" t="s">
@@ -9052,44 +9062,6 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="I194:I195"/>
-    <mergeCell ref="J194:J195"/>
-    <mergeCell ref="H192:H193"/>
-    <mergeCell ref="I192:I193"/>
-    <mergeCell ref="J192:J193"/>
-    <mergeCell ref="A194:A195"/>
-    <mergeCell ref="B194:B195"/>
-    <mergeCell ref="C194:C195"/>
-    <mergeCell ref="D194:D195"/>
-    <mergeCell ref="F194:F195"/>
-    <mergeCell ref="G194:G195"/>
-    <mergeCell ref="H194:H195"/>
-    <mergeCell ref="A192:A193"/>
-    <mergeCell ref="B192:B193"/>
-    <mergeCell ref="C192:C193"/>
-    <mergeCell ref="D192:D193"/>
-    <mergeCell ref="F192:F193"/>
-    <mergeCell ref="G192:G193"/>
-    <mergeCell ref="J125:J126"/>
-    <mergeCell ref="A128:A129"/>
-    <mergeCell ref="B128:B129"/>
-    <mergeCell ref="C128:C129"/>
-    <mergeCell ref="D128:D129"/>
-    <mergeCell ref="F128:F129"/>
-    <mergeCell ref="G128:G129"/>
-    <mergeCell ref="H128:H129"/>
-    <mergeCell ref="I128:I129"/>
-    <mergeCell ref="J128:J129"/>
-    <mergeCell ref="I123:I124"/>
-    <mergeCell ref="J123:J124"/>
-    <mergeCell ref="A125:A126"/>
-    <mergeCell ref="B125:B126"/>
-    <mergeCell ref="C125:C126"/>
-    <mergeCell ref="D125:D126"/>
-    <mergeCell ref="F125:F126"/>
-    <mergeCell ref="G125:G126"/>
-    <mergeCell ref="H125:H126"/>
-    <mergeCell ref="I125:I126"/>
     <mergeCell ref="H50:H51"/>
     <mergeCell ref="I50:I51"/>
     <mergeCell ref="J50:J51"/>
@@ -9106,6 +9078,44 @@
     <mergeCell ref="D50:D51"/>
     <mergeCell ref="F50:F51"/>
     <mergeCell ref="G50:G51"/>
+    <mergeCell ref="I123:I124"/>
+    <mergeCell ref="J123:J124"/>
+    <mergeCell ref="A125:A126"/>
+    <mergeCell ref="B125:B126"/>
+    <mergeCell ref="C125:C126"/>
+    <mergeCell ref="D125:D126"/>
+    <mergeCell ref="F125:F126"/>
+    <mergeCell ref="G125:G126"/>
+    <mergeCell ref="H125:H126"/>
+    <mergeCell ref="I125:I126"/>
+    <mergeCell ref="J125:J126"/>
+    <mergeCell ref="A128:A129"/>
+    <mergeCell ref="B128:B129"/>
+    <mergeCell ref="C128:C129"/>
+    <mergeCell ref="D128:D129"/>
+    <mergeCell ref="F128:F129"/>
+    <mergeCell ref="G128:G129"/>
+    <mergeCell ref="H128:H129"/>
+    <mergeCell ref="I128:I129"/>
+    <mergeCell ref="J128:J129"/>
+    <mergeCell ref="G194:G195"/>
+    <mergeCell ref="H194:H195"/>
+    <mergeCell ref="A192:A193"/>
+    <mergeCell ref="B192:B193"/>
+    <mergeCell ref="C192:C193"/>
+    <mergeCell ref="D192:D193"/>
+    <mergeCell ref="F192:F193"/>
+    <mergeCell ref="G192:G193"/>
+    <mergeCell ref="A194:A195"/>
+    <mergeCell ref="B194:B195"/>
+    <mergeCell ref="C194:C195"/>
+    <mergeCell ref="D194:D195"/>
+    <mergeCell ref="F194:F195"/>
+    <mergeCell ref="I194:I195"/>
+    <mergeCell ref="J194:J195"/>
+    <mergeCell ref="H192:H193"/>
+    <mergeCell ref="I192:I193"/>
+    <mergeCell ref="J192:J193"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
@@ -9304,6 +9314,7 @@
     <hyperlink ref="F200" r:id="rId194"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
semi-final stage of calculating influences
</commit_message>
<xml_diff>
--- a/data/small.xlsx
+++ b/data/small.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2416,7 +2416,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2447,14 +2447,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2473,10 +2465,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2485,11 +2476,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+  <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2823,7 +2813,7 @@
   <dimension ref="A1:J200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J9"/>
+      <selection sqref="A1:J200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4390,7 +4380,7 @@
       <c r="E50" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="F50" s="7" t="s">
+      <c r="F50" s="6" t="s">
         <v>224</v>
       </c>
       <c r="G50" s="5" t="s">
@@ -4402,7 +4392,7 @@
       <c r="I50" s="5">
         <v>123</v>
       </c>
-      <c r="J50" s="6">
+      <c r="J50" s="7">
         <v>40781.633333333331</v>
       </c>
     </row>
@@ -4414,11 +4404,11 @@
       <c r="E51" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="F51" s="7"/>
+      <c r="F51" s="6"/>
       <c r="G51" s="5"/>
       <c r="H51" s="5"/>
       <c r="I51" s="5"/>
-      <c r="J51" s="6"/>
+      <c r="J51" s="7"/>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="1" t="s">
@@ -6690,7 +6680,7 @@
       <c r="E123" s="1" t="s">
         <v>518</v>
       </c>
-      <c r="F123" s="7" t="s">
+      <c r="F123" s="6" t="s">
         <v>519</v>
       </c>
       <c r="G123" s="5" t="s">
@@ -6702,7 +6692,7 @@
       <c r="I123" s="5">
         <v>279</v>
       </c>
-      <c r="J123" s="6">
+      <c r="J123" s="7">
         <v>40781.661805555559</v>
       </c>
     </row>
@@ -6714,11 +6704,11 @@
       <c r="E124" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="F124" s="7"/>
+      <c r="F124" s="6"/>
       <c r="G124" s="5"/>
       <c r="H124" s="5"/>
       <c r="I124" s="5"/>
-      <c r="J124" s="6"/>
+      <c r="J124" s="7"/>
     </row>
     <row r="125" spans="1:10">
       <c r="A125" s="5" t="s">
@@ -6736,7 +6726,7 @@
       <c r="E125" s="1" t="s">
         <v>521</v>
       </c>
-      <c r="F125" s="7" t="s">
+      <c r="F125" s="6" t="s">
         <v>522</v>
       </c>
       <c r="G125" s="5" t="s">
@@ -6748,7 +6738,7 @@
       <c r="I125" s="5">
         <v>279</v>
       </c>
-      <c r="J125" s="6">
+      <c r="J125" s="7">
         <v>40781.661805555559</v>
       </c>
     </row>
@@ -6760,11 +6750,11 @@
       <c r="E126" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="F126" s="7"/>
+      <c r="F126" s="6"/>
       <c r="G126" s="5"/>
       <c r="H126" s="5"/>
       <c r="I126" s="5"/>
-      <c r="J126" s="6"/>
+      <c r="J126" s="7"/>
     </row>
     <row r="127" spans="1:10">
       <c r="A127" s="1" t="s">
@@ -6814,7 +6804,7 @@
       <c r="E128" s="1" t="s">
         <v>528</v>
       </c>
-      <c r="F128" s="7" t="s">
+      <c r="F128" s="6" t="s">
         <v>529</v>
       </c>
       <c r="G128" s="5" t="s">
@@ -6826,7 +6816,7 @@
       <c r="I128" s="5">
         <v>279</v>
       </c>
-      <c r="J128" s="6">
+      <c r="J128" s="7">
         <v>40781.662499999999</v>
       </c>
     </row>
@@ -6838,11 +6828,11 @@
       <c r="E129" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="F129" s="7"/>
+      <c r="F129" s="6"/>
       <c r="G129" s="5"/>
       <c r="H129" s="5"/>
       <c r="I129" s="5"/>
-      <c r="J129" s="6"/>
+      <c r="J129" s="7"/>
     </row>
     <row r="130" spans="1:10">
       <c r="A130" s="1" t="s">
@@ -8828,7 +8818,7 @@
       <c r="E192" s="1" t="s">
         <v>770</v>
       </c>
-      <c r="F192" s="7" t="s">
+      <c r="F192" s="6" t="s">
         <v>771</v>
       </c>
       <c r="G192" s="5" t="s">
@@ -8840,7 +8830,7 @@
       <c r="I192" s="5">
         <v>3931</v>
       </c>
-      <c r="J192" s="6">
+      <c r="J192" s="7">
         <v>40781.681944444441</v>
       </c>
     </row>
@@ -8852,11 +8842,11 @@
       <c r="E193" s="1" t="s">
         <v>772</v>
       </c>
-      <c r="F193" s="7"/>
+      <c r="F193" s="6"/>
       <c r="G193" s="5"/>
       <c r="H193" s="5"/>
       <c r="I193" s="5"/>
-      <c r="J193" s="6"/>
+      <c r="J193" s="7"/>
     </row>
     <row r="194" spans="1:10">
       <c r="A194" s="5" t="s">
@@ -8874,7 +8864,7 @@
       <c r="E194" s="1" t="s">
         <v>775</v>
       </c>
-      <c r="F194" s="7" t="s">
+      <c r="F194" s="6" t="s">
         <v>776</v>
       </c>
       <c r="G194" s="5" t="s">
@@ -8886,7 +8876,7 @@
       <c r="I194" s="5">
         <v>5291</v>
       </c>
-      <c r="J194" s="6">
+      <c r="J194" s="7">
         <v>40781.682638888888</v>
       </c>
     </row>
@@ -8898,11 +8888,11 @@
       <c r="E195" s="1" t="s">
         <v>778</v>
       </c>
-      <c r="F195" s="7"/>
+      <c r="F195" s="6"/>
       <c r="G195" s="5"/>
       <c r="H195" s="5"/>
       <c r="I195" s="5"/>
-      <c r="J195" s="6"/>
+      <c r="J195" s="7"/>
     </row>
     <row r="196" spans="1:10">
       <c r="A196" s="1" t="s">
@@ -9062,6 +9052,44 @@
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="I194:I195"/>
+    <mergeCell ref="J194:J195"/>
+    <mergeCell ref="H192:H193"/>
+    <mergeCell ref="I192:I193"/>
+    <mergeCell ref="J192:J193"/>
+    <mergeCell ref="A194:A195"/>
+    <mergeCell ref="B194:B195"/>
+    <mergeCell ref="C194:C195"/>
+    <mergeCell ref="D194:D195"/>
+    <mergeCell ref="F194:F195"/>
+    <mergeCell ref="G194:G195"/>
+    <mergeCell ref="H194:H195"/>
+    <mergeCell ref="A192:A193"/>
+    <mergeCell ref="B192:B193"/>
+    <mergeCell ref="C192:C193"/>
+    <mergeCell ref="D192:D193"/>
+    <mergeCell ref="F192:F193"/>
+    <mergeCell ref="G192:G193"/>
+    <mergeCell ref="J125:J126"/>
+    <mergeCell ref="A128:A129"/>
+    <mergeCell ref="B128:B129"/>
+    <mergeCell ref="C128:C129"/>
+    <mergeCell ref="D128:D129"/>
+    <mergeCell ref="F128:F129"/>
+    <mergeCell ref="G128:G129"/>
+    <mergeCell ref="H128:H129"/>
+    <mergeCell ref="I128:I129"/>
+    <mergeCell ref="J128:J129"/>
+    <mergeCell ref="I123:I124"/>
+    <mergeCell ref="J123:J124"/>
+    <mergeCell ref="A125:A126"/>
+    <mergeCell ref="B125:B126"/>
+    <mergeCell ref="C125:C126"/>
+    <mergeCell ref="D125:D126"/>
+    <mergeCell ref="F125:F126"/>
+    <mergeCell ref="G125:G126"/>
+    <mergeCell ref="H125:H126"/>
+    <mergeCell ref="I125:I126"/>
     <mergeCell ref="H50:H51"/>
     <mergeCell ref="I50:I51"/>
     <mergeCell ref="J50:J51"/>
@@ -9078,44 +9106,6 @@
     <mergeCell ref="D50:D51"/>
     <mergeCell ref="F50:F51"/>
     <mergeCell ref="G50:G51"/>
-    <mergeCell ref="I123:I124"/>
-    <mergeCell ref="J123:J124"/>
-    <mergeCell ref="A125:A126"/>
-    <mergeCell ref="B125:B126"/>
-    <mergeCell ref="C125:C126"/>
-    <mergeCell ref="D125:D126"/>
-    <mergeCell ref="F125:F126"/>
-    <mergeCell ref="G125:G126"/>
-    <mergeCell ref="H125:H126"/>
-    <mergeCell ref="I125:I126"/>
-    <mergeCell ref="J125:J126"/>
-    <mergeCell ref="A128:A129"/>
-    <mergeCell ref="B128:B129"/>
-    <mergeCell ref="C128:C129"/>
-    <mergeCell ref="D128:D129"/>
-    <mergeCell ref="F128:F129"/>
-    <mergeCell ref="G128:G129"/>
-    <mergeCell ref="H128:H129"/>
-    <mergeCell ref="I128:I129"/>
-    <mergeCell ref="J128:J129"/>
-    <mergeCell ref="G194:G195"/>
-    <mergeCell ref="H194:H195"/>
-    <mergeCell ref="A192:A193"/>
-    <mergeCell ref="B192:B193"/>
-    <mergeCell ref="C192:C193"/>
-    <mergeCell ref="D192:D193"/>
-    <mergeCell ref="F192:F193"/>
-    <mergeCell ref="G192:G193"/>
-    <mergeCell ref="A194:A195"/>
-    <mergeCell ref="B194:B195"/>
-    <mergeCell ref="C194:C195"/>
-    <mergeCell ref="D194:D195"/>
-    <mergeCell ref="F194:F195"/>
-    <mergeCell ref="I194:I195"/>
-    <mergeCell ref="J194:J195"/>
-    <mergeCell ref="H192:H193"/>
-    <mergeCell ref="I192:I193"/>
-    <mergeCell ref="J192:J193"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
@@ -9314,7 +9304,6 @@
     <hyperlink ref="F200" r:id="rId194"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>